<commit_message>
Log file updated, with the links for post36
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>S.No</t>
   </si>
@@ -346,6 +346,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/variables-and-comments-shell-scripting-2e7d</t>
+  </si>
+  <si>
+    <t>Read User Input | Shell Scriptinh</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/read-user-input-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/read-user-input-shell-scripting-4d04</t>
   </si>
 </sst>
 </file>
@@ -559,8 +568,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F45" totalsRowShown="0">
-  <autoFilter ref="B10:F45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F46" totalsRowShown="0">
+  <autoFilter ref="B10:F46">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -859,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F45"/>
+  <dimension ref="B10:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1484,6 +1493,23 @@
       </c>
       <c r="F45" s="5" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="3">
+        <v>36</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="4">
+        <v>44167</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post37
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>S.No</t>
   </si>
@@ -355,6 +355,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/read-user-input-shell-scripting-4d04</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/critical-section-problem-operating-system-mo03-p04-4fhg</t>
+  </si>
+  <si>
+    <t>Critical Section Problem | Operating System - M03 P04</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/critical-section-problem-or-operating-system-m03-p04</t>
   </si>
 </sst>
 </file>
@@ -568,8 +577,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F46" totalsRowShown="0">
-  <autoFilter ref="B10:F46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F47" totalsRowShown="0">
+  <autoFilter ref="B10:F47">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -868,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F46"/>
+  <dimension ref="B10:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1510,6 +1519,23 @@
       </c>
       <c r="F46" s="5" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="B47" s="3">
+        <v>37</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="4">
+        <v>44167</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with the links of Post38
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>S.No</t>
   </si>
@@ -364,6 +364,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/critical-section-problem-or-operating-system-m03-p04</t>
+  </si>
+  <si>
+    <t>Passing Arguments | Shell Scripting</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/passing-arguments-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/passing-arguments-shell-scripting-50</t>
   </si>
 </sst>
 </file>
@@ -577,8 +586,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F47" totalsRowShown="0">
-  <autoFilter ref="B10:F47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F48" totalsRowShown="0">
+  <autoFilter ref="B10:F48">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -877,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F47"/>
+  <dimension ref="B10:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1536,6 +1545,23 @@
       </c>
       <c r="F47" s="5" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="3">
+        <v>38</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="4">
+        <v>44168</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, wiht the link of Post39
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>S.No</t>
   </si>
@@ -373,6 +373,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/passing-arguments-shell-scripting-50</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/if-statement-or-shell-scripting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If Statement | Shell Scripting </t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/if-statement-shell-scripting-434j</t>
   </si>
 </sst>
 </file>
@@ -586,8 +595,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F48" totalsRowShown="0">
-  <autoFilter ref="B10:F48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F49" totalsRowShown="0">
+  <autoFilter ref="B10:F49">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -886,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F48"/>
+  <dimension ref="B10:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1562,6 +1571,23 @@
       </c>
       <c r="F48" s="5" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="3">
+        <v>39</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="4">
+        <v>44168</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post40
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>S.No</t>
   </si>
@@ -382,6 +382,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/if-statement-shell-scripting-434j</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/semaphores-and-counting-semaphores-operating-system-m03-p05-3fbo</t>
+  </si>
+  <si>
+    <t>Semaphores and Counting Semaphores | Operating System - M03 P05</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/semaphores-and-counting-semaphores-or-operating-system-m03-p05</t>
   </si>
 </sst>
 </file>
@@ -595,8 +604,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F49" totalsRowShown="0">
-  <autoFilter ref="B10:F49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F50" totalsRowShown="0">
+  <autoFilter ref="B10:F50">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -895,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F49"/>
+  <dimension ref="B10:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1588,6 +1597,23 @@
       </c>
       <c r="F49" s="5" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50" s="3">
+        <v>40</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="4">
+        <v>44168</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post41
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>S.No</t>
   </si>
@@ -391,6 +391,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/semaphores-and-counting-semaphores-or-operating-system-m03-p05</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/file-test-operator-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>File Test Operator | Shell Scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/file-test-operator-shell-scripting-2hha</t>
   </si>
 </sst>
 </file>
@@ -604,8 +613,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F50" totalsRowShown="0">
-  <autoFilter ref="B10:F50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F51" totalsRowShown="0">
+  <autoFilter ref="B10:F51">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -904,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F50"/>
+  <dimension ref="B10:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1614,6 +1623,23 @@
       </c>
       <c r="F50" s="5" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51" s="3">
+        <v>41</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="4">
+        <v>44169</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post42
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>S.No</t>
   </si>
@@ -400,6 +400,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/file-test-operator-shell-scripting-2hha</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/binary-semaphore-operating-system-m03-p06-2l08</t>
+  </si>
+  <si>
+    <t>Binary Semaphore | Operating System - M03 P06</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/binary-semaphore-or-operating-system-m03-p06</t>
   </si>
 </sst>
 </file>
@@ -613,8 +622,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F51" totalsRowShown="0">
-  <autoFilter ref="B10:F51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F52" totalsRowShown="0">
+  <autoFilter ref="B10:F52">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -913,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F51"/>
+  <dimension ref="B10:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1640,6 +1649,23 @@
       </c>
       <c r="F51" s="5" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="3">
+        <v>42</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="4">
+        <v>44169</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post43
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>S.No</t>
   </si>
@@ -409,6 +409,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/binary-semaphore-or-operating-system-m03-p06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Append Data in File | Shell Scripting </t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/append-data-in-file-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/append-data-in-file-shell-scripting-ne0</t>
   </si>
 </sst>
 </file>
@@ -622,8 +631,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F52" totalsRowShown="0">
-  <autoFilter ref="B10:F52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F53" totalsRowShown="0">
+  <autoFilter ref="B10:F53">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -922,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F52"/>
+  <dimension ref="B10:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1666,6 +1675,23 @@
       </c>
       <c r="F52" s="5" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="3">
+        <v>43</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="4">
+        <v>44170</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post44
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t>S.No</t>
   </si>
@@ -418,6 +418,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/append-data-in-file-shell-scripting-ne0</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/logical-and-operator-or-shell-scripting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logical 'AND' Operator | Shell Scripting </t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/logical-and-operator-shell-scripting-9cg</t>
   </si>
 </sst>
 </file>
@@ -631,8 +640,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F53" totalsRowShown="0">
-  <autoFilter ref="B10:F53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F54" totalsRowShown="0">
+  <autoFilter ref="B10:F54">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -931,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F53"/>
+  <dimension ref="B10:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1692,6 +1701,23 @@
       </c>
       <c r="F53" s="5" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="3">
+        <v>44</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D54" s="4">
+        <v>44170</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post45
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>S.No</t>
   </si>
@@ -427,6 +427,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/logical-and-operator-shell-scripting-9cg</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/question-on-binary-semaphore-operating-system-m03-p07-3alp</t>
+  </si>
+  <si>
+    <t>Question on Binary Semaphore | Operating System - M03 P07</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/question-on-binary-semaphore-or-operating-system-m03-p07</t>
   </si>
 </sst>
 </file>
@@ -640,8 +649,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F54" totalsRowShown="0">
-  <autoFilter ref="B10:F54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F55" totalsRowShown="0">
+  <autoFilter ref="B10:F55">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -940,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F54"/>
+  <dimension ref="B10:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1718,6 +1727,23 @@
       </c>
       <c r="F54" s="5" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="3">
+        <v>45</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" s="4">
+        <v>44170</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post46
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
   <si>
     <t>S.No</t>
   </si>
@@ -436,6 +436,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/question-on-binary-semaphore-or-operating-system-m03-p07</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/dining-philosopher-problem-operating-system-m03-p08-fa5</t>
+  </si>
+  <si>
+    <t>Dining Philosopher problem | Operating System - M03 P08</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/dining-philosopher-problem-or-operating-system-m03-p08</t>
   </si>
 </sst>
 </file>
@@ -649,8 +658,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F55" totalsRowShown="0">
-  <autoFilter ref="B10:F55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F56" totalsRowShown="0">
+  <autoFilter ref="B10:F56">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -949,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F55"/>
+  <dimension ref="B10:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1744,6 +1753,23 @@
       </c>
       <c r="F55" s="5" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56" s="3">
+        <v>46</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D56" s="4">
+        <v>44171</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with the links of Post47
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>S.No</t>
   </si>
@@ -445,6 +445,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/dining-philosopher-problem-or-operating-system-m03-p08</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/logical-or-operator-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/logical-or-operator-shell-scripting-57gm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logical 'OR' Operator | Shell Scripting </t>
   </si>
 </sst>
 </file>
@@ -658,8 +667,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F56" totalsRowShown="0">
-  <autoFilter ref="B10:F56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F57" totalsRowShown="0">
+  <autoFilter ref="B10:F57">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -958,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F56"/>
+  <dimension ref="B10:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1770,6 +1779,23 @@
       </c>
       <c r="F56" s="5" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="3">
+        <v>47</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D57" s="4">
+        <v>44172</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with the likns of Post48
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t>S.No</t>
   </si>
@@ -454,6 +454,15 @@
   </si>
   <si>
     <t xml:space="preserve">Logical 'OR' Operator | Shell Scripting </t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/deadlock-operating-system-m04-p01-5c92</t>
+  </si>
+  <si>
+    <t>Deadlock | Operating System - M04 P01</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/deadlock-or-operating-system-m04-p01</t>
   </si>
 </sst>
 </file>
@@ -667,8 +676,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F57" totalsRowShown="0">
-  <autoFilter ref="B10:F57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F58" totalsRowShown="0">
+  <autoFilter ref="B10:F58">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -967,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F57"/>
+  <dimension ref="B10:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1796,6 +1805,23 @@
       </c>
       <c r="F57" s="5" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58" s="3">
+        <v>48</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D58" s="4">
+        <v>44172</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post49
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>S.No</t>
   </si>
@@ -463,6 +463,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/deadlock-or-operating-system-m04-p01</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/resource-allocation-graph-in-deadlock-operating-system-m04-p02-568p</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/resource-allocation-graph-in-deadlock-or-operating-system-m04-p02</t>
+  </si>
+  <si>
+    <t>Resource Allocation Graph in Deadlock | Operating System - M04 P02</t>
   </si>
 </sst>
 </file>
@@ -676,8 +685,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F58" totalsRowShown="0">
-  <autoFilter ref="B10:F58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F59" totalsRowShown="0">
+  <autoFilter ref="B10:F59">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -976,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F58"/>
+  <dimension ref="B10:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1822,6 +1831,23 @@
       </c>
       <c r="F58" s="5" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="B59" s="3">
+        <v>49</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D59" s="4">
+        <v>44173</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post50
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>S.No</t>
   </si>
@@ -472,6 +472,15 @@
   </si>
   <si>
     <t>Resource Allocation Graph in Deadlock | Operating System - M04 P02</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/arithmetic-operations-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/arithmetic-operations-shell-scripting-340j</t>
+  </si>
+  <si>
+    <t>Arithmetic Operations | Shell Scripting</t>
   </si>
 </sst>
 </file>
@@ -685,8 +694,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F59" totalsRowShown="0">
-  <autoFilter ref="B10:F59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F60" totalsRowShown="0">
+  <autoFilter ref="B10:F60">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -985,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F59"/>
+  <dimension ref="B10:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1848,6 +1857,23 @@
       </c>
       <c r="F59" s="5" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="B60" s="3">
+        <v>50</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D60" s="4">
+        <v>44174</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post51
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>S.No</t>
   </si>
@@ -481,6 +481,15 @@
   </si>
   <si>
     <t>Arithmetic Operations | Shell Scripting</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/floating-point-operations-or-shell-scripting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floating Point Operations | Shell Scripting </t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/floating-point-operations-shell-scripting-4hk0</t>
   </si>
 </sst>
 </file>
@@ -694,8 +703,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F60" totalsRowShown="0">
-  <autoFilter ref="B10:F60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F61" totalsRowShown="0">
+  <autoFilter ref="B10:F61">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -994,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F60"/>
+  <dimension ref="B10:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1874,6 +1883,23 @@
       </c>
       <c r="F60" s="5" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6">
+      <c r="B61" s="3">
+        <v>51</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D61" s="4">
+        <v>44174</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post52
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
   <si>
     <t>S.No</t>
   </si>
@@ -490,6 +490,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/floating-point-operations-shell-scripting-4hk0</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/multi-instance-resource-allocation-graph-operating-system-m04-p03-15nh</t>
+  </si>
+  <si>
+    <t>Multi-Instance Resource Allocation Graph | Operating System - M04 P03</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/multi-instance-resource-allocation-graph-or-operating-system-m04-p03</t>
   </si>
 </sst>
 </file>
@@ -703,8 +712,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F61" totalsRowShown="0">
-  <autoFilter ref="B10:F61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F62" totalsRowShown="0">
+  <autoFilter ref="B10:F62">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1003,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F61"/>
+  <dimension ref="B10:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1900,6 +1909,23 @@
       </c>
       <c r="F61" s="5" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6">
+      <c r="B62" s="3">
+        <v>52</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D62" s="4">
+        <v>44174</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post53
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>S.No</t>
   </si>
@@ -499,6 +499,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/multi-instance-resource-allocation-graph-or-operating-system-m04-p03</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/deadlock-prevention-operating-system-m04-p04-4khe</t>
+  </si>
+  <si>
+    <t>Deadlock Prevention | Operating System - M04 P04</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/deadlock-prevention-or-operating-system-m04-p04</t>
   </si>
 </sst>
 </file>
@@ -712,8 +721,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F62" totalsRowShown="0">
-  <autoFilter ref="B10:F62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F63" totalsRowShown="0">
+  <autoFilter ref="B10:F63">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1012,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F62"/>
+  <dimension ref="B10:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1926,6 +1935,23 @@
       </c>
       <c r="F62" s="5" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63" s="3">
+        <v>53</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D63" s="4">
+        <v>44175</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post54
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
   <si>
     <t>S.No</t>
   </si>
@@ -508,6 +508,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/deadlock-prevention-or-operating-system-m04-p04</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/deadlock-avoidance-banker-s-algorithm-operating-system-m04-p05-4fgk</t>
+  </si>
+  <si>
+    <t>Deadlock Avoidance (Banker's Algorithm) | Operating System - M04 P05</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/deadlock-avoidance-bankers-algorithm-or-operating-system-m04-p05</t>
   </si>
 </sst>
 </file>
@@ -721,8 +730,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F63" totalsRowShown="0">
-  <autoFilter ref="B10:F63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F64" totalsRowShown="0">
+  <autoFilter ref="B10:F64">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1021,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F63"/>
+  <dimension ref="B10:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1952,6 +1961,23 @@
       </c>
       <c r="F63" s="5" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64" s="3">
+        <v>54</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D64" s="4">
+        <v>44176</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post55
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>S.No</t>
   </si>
@@ -517,6 +517,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/deadlock-avoidance-bankers-algorithm-or-operating-system-m04-p05</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/case-statement-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/case-statement-shell-scripting-2o2a</t>
+  </si>
+  <si>
+    <t>Case Statement | Shell Scripting</t>
   </si>
 </sst>
 </file>
@@ -730,8 +739,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F64" totalsRowShown="0">
-  <autoFilter ref="B10:F64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F65" totalsRowShown="0">
+  <autoFilter ref="B10:F65">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1030,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F64"/>
+  <dimension ref="B10:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1978,6 +1987,23 @@
       </c>
       <c r="F64" s="5" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="3">
+        <v>55</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D65" s="4">
+        <v>44177</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post56
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t>S.No</t>
   </si>
@@ -526,6 +526,15 @@
   </si>
   <si>
     <t>Case Statement | Shell Scripting</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/case-statement-example-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/case-statement-example-shell-scripting-2gmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case Statement Example | Shell Scrtipting </t>
   </si>
 </sst>
 </file>
@@ -739,8 +748,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F65" totalsRowShown="0">
-  <autoFilter ref="B10:F65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F66" totalsRowShown="0">
+  <autoFilter ref="B10:F66">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1039,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F65"/>
+  <dimension ref="B10:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F43" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2004,6 +2013,23 @@
       </c>
       <c r="F65" s="5" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66" s="3">
+        <v>56</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D66" s="4">
+        <v>44177</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LOg file updated, with loinks of Post57
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
   <si>
     <t>S.No</t>
   </si>
@@ -535,6 +535,15 @@
   </si>
   <si>
     <t xml:space="preserve">Case Statement Example | Shell Scrtipting </t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/banker-s-algorithm-question-operating-system-m04-p06-3lgj</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/bankers-algorithm-question-or-operating-system-m04-p06</t>
+  </si>
+  <si>
+    <t>Banker's Algorithm Question | Operating System - Mo4 P06</t>
   </si>
 </sst>
 </file>
@@ -748,8 +757,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F66" totalsRowShown="0">
-  <autoFilter ref="B10:F66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F67" totalsRowShown="0">
+  <autoFilter ref="B10:F67">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1048,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F66"/>
+  <dimension ref="B10:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2030,6 +2039,23 @@
       </c>
       <c r="F66" s="5" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67" s="3">
+        <v>57</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D67" s="4">
+        <v>44177</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post58
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
   <si>
     <t>S.No</t>
   </si>
@@ -544,6 +544,15 @@
   </si>
   <si>
     <t>Banker's Algorithm Question | Operating System - Mo4 P06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Array variable | Shell Scripting </t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/array-variable-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/array-variable-shell-scripting-56c3</t>
   </si>
 </sst>
 </file>
@@ -757,8 +766,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F67" totalsRowShown="0">
-  <autoFilter ref="B10:F67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F68" totalsRowShown="0">
+  <autoFilter ref="B10:F68">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1057,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F67"/>
+  <dimension ref="B10:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="F51" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2056,6 +2065,23 @@
       </c>
       <c r="F67" s="5" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="3">
+        <v>58</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D68" s="4">
+        <v>44178</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post59
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t>S.No</t>
   </si>
@@ -553,6 +553,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/array-variable-shell-scripting-56c3</t>
+  </si>
+  <si>
+    <t>While Loop | Shell Scripting</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/while-loop-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/while-loop-shell-scripting-5f9a</t>
   </si>
 </sst>
 </file>
@@ -766,8 +775,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F68" totalsRowShown="0">
-  <autoFilter ref="B10:F68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F69" totalsRowShown="0">
+  <autoFilter ref="B10:F69">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1066,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F68"/>
+  <dimension ref="B10:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F51" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2082,6 +2091,23 @@
       </c>
       <c r="F68" s="5" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69" s="3">
+        <v>59</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D69" s="4">
+        <v>44178</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post60
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>S.No</t>
   </si>
@@ -543,9 +543,6 @@
     <t>https://programmingport.hashnode.dev/bankers-algorithm-question-or-operating-system-m04-p06</t>
   </si>
   <si>
-    <t>Banker's Algorithm Question | Operating System - Mo4 P06</t>
-  </si>
-  <si>
     <t xml:space="preserve">Array variable | Shell Scripting </t>
   </si>
   <si>
@@ -562,6 +559,18 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/while-loop-shell-scripting-5f9a</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/question-on-deadlock-operating-system-m04-p07-37hh</t>
+  </si>
+  <si>
+    <t>Question on Deadlock | Operating System - M04 P07</t>
+  </si>
+  <si>
+    <t>Banker's Algorithm Question | Operating System - M04 P06</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/question-on-deadlock-or-operating-system-m04-p07</t>
   </si>
 </sst>
 </file>
@@ -775,8 +784,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F69" totalsRowShown="0">
-  <autoFilter ref="B10:F69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F70" totalsRowShown="0">
+  <autoFilter ref="B10:F70">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1075,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F69"/>
+  <dimension ref="B10:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F51" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="D51" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2064,7 +2073,7 @@
         <v>57</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D67" s="4">
         <v>44177</v>
@@ -2081,16 +2090,16 @@
         <v>58</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D68" s="4">
         <v>44178</v>
       </c>
       <c r="E68" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="F68" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -2098,15 +2107,32 @@
         <v>59</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D69" s="4">
         <v>44178</v>
       </c>
       <c r="E69" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F69" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="F69" s="5" t="s">
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" s="3">
+        <v>60</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D70" s="4">
+        <v>44178</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F70" s="5" t="s">
         <v>181</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Log file updated, with links of Post61
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
   <si>
     <t>S.No</t>
   </si>
@@ -571,6 +571,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/question-on-deadlock-or-operating-system-m04-p07</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/sleep-and-open-terminal-using-while-loop-or-shell-scripting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleep and Open Terminal using While Loop | Shell Scripting </t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/sleep-and-open-terminal-using-while-loop-shell-scripting-2mea</t>
   </si>
 </sst>
 </file>
@@ -784,8 +793,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F70" totalsRowShown="0">
-  <autoFilter ref="B10:F70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F71" totalsRowShown="0">
+  <autoFilter ref="B10:F71">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1084,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F70"/>
+  <dimension ref="B10:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D51" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="F51" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2134,6 +2143,23 @@
       </c>
       <c r="F70" s="5" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" s="3">
+        <v>61</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D71" s="4">
+        <v>44179</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post62
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
   <si>
     <t>S.No</t>
   </si>
@@ -580,6 +580,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/sleep-and-open-terminal-using-while-loop-shell-scripting-2mea</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/read-files-content-using-while-loop-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>Read File's Content using While Loop | Shell Scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/read-file-s-content-using-while-loop-shell-scripting-2anl</t>
   </si>
 </sst>
 </file>
@@ -793,8 +802,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F71" totalsRowShown="0">
-  <autoFilter ref="B10:F71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F72" totalsRowShown="0">
+  <autoFilter ref="B10:F72">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1093,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F71"/>
+  <dimension ref="B10:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F51" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2160,6 +2169,23 @@
       </c>
       <c r="F71" s="5" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72" s="3">
+        <v>62</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D72" s="4">
+        <v>44179</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post63
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
   <si>
     <t>S.No</t>
   </si>
@@ -589,6 +589,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/read-file-s-content-using-while-loop-shell-scripting-2anl</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/question-on-deadlock-operating-system-m04-p08-353n</t>
+  </si>
+  <si>
+    <t>Question on Deadlock | Operating System - M04 P08</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/question-on-deadlock-or-operating-system-m04-p08</t>
   </si>
 </sst>
 </file>
@@ -802,8 +811,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F72" totalsRowShown="0">
-  <autoFilter ref="B10:F72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F73" totalsRowShown="0">
+  <autoFilter ref="B10:F73">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1102,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F72"/>
+  <dimension ref="B10:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F51" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" topLeftCell="D51" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2186,6 +2195,23 @@
       </c>
       <c r="F72" s="5" t="s">
         <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" s="3">
+        <v>63</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D73" s="4">
+        <v>44179</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log files updated, with links of Post64
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="197">
   <si>
     <t>S.No</t>
   </si>
@@ -598,6 +598,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/question-on-deadlock-or-operating-system-m04-p08</t>
+  </si>
+  <si>
+    <t>https://hashnode.com/draft/5fd805cd7418a90e83c89a75</t>
+  </si>
+  <si>
+    <t>Until Loop | Shell Scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/until-loop-shell-scripting-4b8o</t>
   </si>
 </sst>
 </file>
@@ -811,8 +820,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F73" totalsRowShown="0">
-  <autoFilter ref="B10:F73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F74" totalsRowShown="0">
+  <autoFilter ref="B10:F74">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1111,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F73"/>
+  <dimension ref="B10:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D51" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="F63" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2212,6 +2221,23 @@
       </c>
       <c r="F73" s="5" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74" s="3">
+        <v>64</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D74" s="4">
+        <v>44180</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Link of Post64 for hashnod updated.
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -600,13 +600,13 @@
     <t>https://programmingport.hashnode.dev/question-on-deadlock-or-operating-system-m04-p08</t>
   </si>
   <si>
-    <t>https://hashnode.com/draft/5fd805cd7418a90e83c89a75</t>
-  </si>
-  <si>
     <t>Until Loop | Shell Scripting</t>
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/until-loop-shell-scripting-4b8o</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/until-loop-or-shell-scripting</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B10:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F63" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="D63" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2228,16 +2228,16 @@
         <v>64</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D74" s="4">
         <v>44180</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file upated, with links of Post65
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>S.No</t>
   </si>
@@ -607,6 +607,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/until-loop-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/for-loop-or-shell-scripting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Loop | Shell Scripting </t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/for-loop-shell-scripting-564f</t>
   </si>
 </sst>
 </file>
@@ -820,8 +829,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F74" totalsRowShown="0">
-  <autoFilter ref="B10:F74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F75" totalsRowShown="0">
+  <autoFilter ref="B10:F75">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1120,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F74"/>
+  <dimension ref="B10:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D63" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" topLeftCell="F63" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2238,6 +2247,23 @@
       </c>
       <c r="F74" s="5" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" s="3">
+        <v>65</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D75" s="4">
+        <v>44180</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post66
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
   <si>
     <t>S.No</t>
   </si>
@@ -616,6 +616,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/for-loop-shell-scripting-564f</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/memory-management-and-degree-of-multiprogramming-operating-system-m05-p01-4fhp</t>
+  </si>
+  <si>
+    <t>Memory Management and Degree of Multiprogramming | Ooerating System - M05 P01</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/memory-management-and-degree-of-multiprogramming-or-operating-system-m05-p01</t>
   </si>
 </sst>
 </file>
@@ -829,8 +838,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F75" totalsRowShown="0">
-  <autoFilter ref="B10:F75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F76" totalsRowShown="0">
+  <autoFilter ref="B10:F76">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1129,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F75"/>
+  <dimension ref="B10:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F63" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="D63" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2264,6 +2273,23 @@
       </c>
       <c r="F75" s="5" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6">
+      <c r="B76" s="3">
+        <v>66</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D76" s="4">
+        <v>44180</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post67
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
   <si>
     <t>S.No</t>
   </si>
@@ -625,6 +625,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/memory-management-and-degree-of-multiprogramming-or-operating-system-m05-p01</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/memory-management-techniques-operating-system-m05-p02-2ei1</t>
+  </si>
+  <si>
+    <t>Memory management Techniques | Operating System - M05 P02</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/memory-management-techniques-or-operating-system-m05-p02-1</t>
   </si>
 </sst>
 </file>
@@ -838,8 +847,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F76" totalsRowShown="0">
-  <autoFilter ref="B10:F76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F77" totalsRowShown="0">
+  <autoFilter ref="B10:F77">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1138,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F76"/>
+  <dimension ref="B10:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D63" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2290,6 +2299,23 @@
       </c>
       <c r="F76" s="5" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="B77" s="3">
+        <v>67</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D77" s="4">
+        <v>44181</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post68
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="209">
   <si>
     <t>S.No</t>
   </si>
@@ -634,6 +634,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/memory-management-techniques-or-operating-system-m05-p02-1</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/for-loop-to-execute-commands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Loop to Execute Commands | Shell Scripting </t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/for-loop-to-execute-commands-shell-scripting-1kak</t>
   </si>
 </sst>
 </file>
@@ -847,8 +856,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F77" totalsRowShown="0">
-  <autoFilter ref="B10:F77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F78" totalsRowShown="0">
+  <autoFilter ref="B10:F78">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1147,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F77"/>
+  <dimension ref="B10:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D63" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="F63" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2316,6 +2325,23 @@
       </c>
       <c r="F77" s="5" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="B78" s="3">
+        <v>68</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D78" s="4">
+        <v>44182</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post69
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
   <si>
     <t>S.No</t>
   </si>
@@ -643,6 +643,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/for-loop-to-execute-commands-shell-scripting-1kak</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/select-loop-or-shell-scripting</t>
+  </si>
+  <si>
+    <t>Select Loop | Shell Scripting</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/select-loop-shell-scripting-3lme</t>
   </si>
 </sst>
 </file>
@@ -856,8 +865,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F78" totalsRowShown="0">
-  <autoFilter ref="B10:F78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F79" totalsRowShown="0">
+  <autoFilter ref="B10:F79">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1156,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F78"/>
+  <dimension ref="B10:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F63" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2342,6 +2351,23 @@
       </c>
       <c r="F78" s="5" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6">
+      <c r="B79" s="3">
+        <v>69</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D79" s="4">
+        <v>44182</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post70
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
   <si>
     <t>S.No</t>
   </si>
@@ -652,6 +652,15 @@
   </si>
   <si>
     <t>https://dev.to/rahulmishra05/select-loop-shell-scripting-3lme</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/fixed-partition-operating-system-m05-p03-4lmm</t>
+  </si>
+  <si>
+    <t>Fixed Partition | Operating System - M05 P03</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/fixed-partition-or-operating-system-m05-p03</t>
   </si>
 </sst>
 </file>
@@ -865,8 +874,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F79" totalsRowShown="0">
-  <autoFilter ref="B10:F79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F80" totalsRowShown="0">
+  <autoFilter ref="B10:F80">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1165,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F79"/>
+  <dimension ref="B10:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F63" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView tabSelected="1" topLeftCell="D63" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2368,6 +2377,23 @@
       </c>
       <c r="F79" s="5" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6">
+      <c r="B80" s="3">
+        <v>70</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D80" s="4">
+        <v>44182</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post71
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
   <si>
     <t>S.No</t>
   </si>
@@ -661,6 +661,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/fixed-partition-or-operating-system-m05-p03</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/variable-partitioning-operating-system-m05-p04-3g9a</t>
+  </si>
+  <si>
+    <t>Variable Partitioning | Operating System - M05 P04</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/variable-partitioning-or-operating-system-m05-p04</t>
   </si>
 </sst>
 </file>
@@ -874,8 +883,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F80" totalsRowShown="0">
-  <autoFilter ref="B10:F80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F81" totalsRowShown="0">
+  <autoFilter ref="B10:F81">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1174,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F80"/>
+  <dimension ref="B10:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D63" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2394,6 +2403,23 @@
       </c>
       <c r="F80" s="5" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="B81" s="3">
+        <v>71</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D81" s="4">
+        <v>44183</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post72
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
   <si>
     <t>S.No</t>
   </si>
@@ -670,6 +670,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/variable-partitioning-or-operating-system-m05-p04</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/various-allocation-methods-in-contiguous-memory-management-operating-system-m05-p05-1k1c</t>
+  </si>
+  <si>
+    <t>Various Allocation Methods in Contiguous Memory Management | Operating System - M05 P05</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/various-allocation-methods-in-contiguous-memory-management-or-operating-system-m05-p05</t>
   </si>
 </sst>
 </file>
@@ -883,8 +892,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F81" totalsRowShown="0">
-  <autoFilter ref="B10:F81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F82" totalsRowShown="0">
+  <autoFilter ref="B10:F82">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1183,16 +1192,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F81"/>
+  <dimension ref="B10:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D63" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="D67" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="10.26953125" customWidth="1"/>
-    <col min="3" max="3" width="73.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.54296875" customWidth="1"/>
     <col min="4" max="4" width="17.36328125" customWidth="1"/>
     <col min="5" max="5" width="116" customWidth="1"/>
     <col min="6" max="6" width="133.6328125" customWidth="1"/>
@@ -2420,6 +2429,23 @@
       </c>
       <c r="F81" s="5" t="s">
         <v>215</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6">
+      <c r="B82" s="3">
+        <v>72</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D82" s="4">
+        <v>44184</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post73
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
   <si>
     <t>S.No</t>
   </si>
@@ -679,6 +679,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/various-allocation-methods-in-contiguous-memory-management-or-operating-system-m05-p05</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/question-on-contiguous-memory-management-operating-system-m05-p06-df5</t>
+  </si>
+  <si>
+    <t>Question on Contiguous Memory Management | Operating System - M05 P06</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/question-on-contiguous-memory-management-or-operating-system-m05-p06</t>
   </si>
 </sst>
 </file>
@@ -892,8 +901,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F82" totalsRowShown="0">
-  <autoFilter ref="B10:F82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F83" totalsRowShown="0">
+  <autoFilter ref="B10:F83">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1192,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F82"/>
+  <dimension ref="B10:F83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D67" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2446,6 +2455,23 @@
       </c>
       <c r="F82" s="5" t="s">
         <v>218</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6">
+      <c r="B83" s="3">
+        <v>73</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D83" s="4">
+        <v>44185</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post74
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="227">
   <si>
     <t>S.No</t>
   </si>
@@ -688,6 +688,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/question-on-contiguous-memory-management-or-operating-system-m05-p06</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/question-on-contiguous-memory-management-operating-system-m05-p07-4kb1</t>
+  </si>
+  <si>
+    <t>Question on Contiguous Memory Management | Operating System - M05 P07</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/question-on-contiguous-memory-management-or-operating-system-m05-p07</t>
   </si>
 </sst>
 </file>
@@ -901,8 +910,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F83" totalsRowShown="0">
-  <autoFilter ref="B10:F83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F84" totalsRowShown="0">
+  <autoFilter ref="B10:F84">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1201,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F83"/>
+  <dimension ref="B10:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D67" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2472,6 +2481,23 @@
       </c>
       <c r="F83" s="5" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6">
+      <c r="B84" s="3">
+        <v>74</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D84" s="4">
+        <v>44186</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post75
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
   <si>
     <t>S.No</t>
   </si>
@@ -697,6 +697,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/question-on-contiguous-memory-management-or-operating-system-m05-p07</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/non-contiguous-memory-allocation-operating-system-m05-p08-56ep</t>
+  </si>
+  <si>
+    <t>Non-Contiguous Memory Management | Operating System - M05 P08</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/non-contiguous-memory-allocation-or-operating-system-m05-p08</t>
   </si>
 </sst>
 </file>
@@ -910,8 +919,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F84" totalsRowShown="0">
-  <autoFilter ref="B10:F84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F85" totalsRowShown="0">
+  <autoFilter ref="B10:F85">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1210,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F84"/>
+  <dimension ref="B10:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D67" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2498,6 +2507,23 @@
       </c>
       <c r="F84" s="5" t="s">
         <v>224</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6">
+      <c r="B85" s="3">
+        <v>75</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D85" s="4">
+        <v>44187</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file upadted, with links of POst76
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="233">
   <si>
     <t>S.No</t>
   </si>
@@ -706,6 +706,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/non-contiguous-memory-allocation-or-operating-system-m05-p08</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/paging-operating-system-m05-p09-25c2</t>
+  </si>
+  <si>
+    <t>Paging | Operating System - M05 P09</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/paging-or-operating-system-m05-p09</t>
   </si>
 </sst>
 </file>
@@ -919,8 +928,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F85" totalsRowShown="0">
-  <autoFilter ref="B10:F85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F86" totalsRowShown="0">
+  <autoFilter ref="B10:F86">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1219,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F85"/>
+  <dimension ref="B10:F86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D67" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2524,6 +2533,23 @@
       </c>
       <c r="F85" s="5" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6">
+      <c r="B86" s="3">
+        <v>76</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D86" s="4">
+        <v>44188</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post77
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
   <si>
     <t>S.No</t>
   </si>
@@ -715,6 +715,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/paging-or-operating-system-m05-p09</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/question-on-logical-address-physical-address-operating-system-m05-p10-pmb</t>
+  </si>
+  <si>
+    <t>Question on Logical Address &amp; Physical Address | Operating System - M05 P10</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/question-on-logical-address-and-physical-address-or-operating-system-m05-p10</t>
   </si>
 </sst>
 </file>
@@ -928,8 +937,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F86" totalsRowShown="0">
-  <autoFilter ref="B10:F86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F87" totalsRowShown="0">
+  <autoFilter ref="B10:F87">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1228,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F86"/>
+  <dimension ref="B10:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D67" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2550,6 +2559,23 @@
       </c>
       <c r="F86" s="5" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6">
+      <c r="B87" s="3">
+        <v>77</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D87" s="4">
+        <v>44189</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post78
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="239">
   <si>
     <t>S.No</t>
   </si>
@@ -724,6 +724,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/question-on-logical-address-and-physical-address-or-operating-system-m05-p10</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/question-on-logical-address-physical-address-operating-system-m05-p11-21n5</t>
+  </si>
+  <si>
+    <t>Question on Logical Address &amp; Physical Address | Operating System - M05 P11</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/question-on-logical-address-and-physical-address-or-operating-system-m05-p11</t>
   </si>
 </sst>
 </file>
@@ -937,8 +946,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F87" totalsRowShown="0">
-  <autoFilter ref="B10:F87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F88" totalsRowShown="0">
+  <autoFilter ref="B10:F88">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1237,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F87"/>
+  <dimension ref="B10:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D67" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2576,6 +2585,23 @@
       </c>
       <c r="F87" s="5" t="s">
         <v>233</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6">
+      <c r="B88" s="3">
+        <v>78</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D88" s="4">
+        <v>44190</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post79
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
   <si>
     <t>S.No</t>
   </si>
@@ -733,6 +733,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/question-on-logical-address-and-physical-address-or-operating-system-m05-p11</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/page-table-entry-operating-system-m05-p12-5hi0</t>
+  </si>
+  <si>
+    <t>Page Table Entry | Operating System - M05 P12</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/page-table-entry-or-operating-system-m05-p12</t>
   </si>
 </sst>
 </file>
@@ -946,8 +955,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F88" totalsRowShown="0">
-  <autoFilter ref="B10:F88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F89" totalsRowShown="0">
+  <autoFilter ref="B10:F89">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1246,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F88"/>
+  <dimension ref="B10:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D67" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2602,6 +2611,23 @@
       </c>
       <c r="F88" s="5" t="s">
         <v>236</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6">
+      <c r="B89" s="3">
+        <v>79</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D89" s="4">
+        <v>44191</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post80
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
   <si>
     <t>S.No</t>
   </si>
@@ -742,6 +742,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/page-table-entry-or-operating-system-m05-p12</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/2-level-paging-operating-system-m05-p13-3f0n</t>
+  </si>
+  <si>
+    <t>2-Level Paging | Operating System - M05 P13</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/2-level-paging-or-operating-system-m05-p13</t>
   </si>
 </sst>
 </file>
@@ -955,8 +964,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F89" totalsRowShown="0">
-  <autoFilter ref="B10:F89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F90" totalsRowShown="0">
+  <autoFilter ref="B10:F90">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1255,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F89"/>
+  <dimension ref="B10:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D67" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" topLeftCell="D82" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2628,6 +2637,23 @@
       </c>
       <c r="F89" s="5" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6">
+      <c r="B90" s="3">
+        <v>80</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D90" s="4">
+        <v>44193</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LOg file updated, with links of Post81
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="248">
   <si>
     <t>S.No</t>
   </si>
@@ -751,6 +751,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/2-level-paging-or-operating-system-m05-p13</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/inverted-paging-operating-system-m05-p14-2nd7</t>
+  </si>
+  <si>
+    <t>Inverted Paging | Operating System - M05 P14</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/inverted-paging-or-operating-system-m05-p14</t>
   </si>
 </sst>
 </file>
@@ -964,8 +973,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F90" totalsRowShown="0">
-  <autoFilter ref="B10:F90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F91" totalsRowShown="0">
+  <autoFilter ref="B10:F91">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1264,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F90"/>
+  <dimension ref="B10:F91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D82" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2654,6 +2663,23 @@
       </c>
       <c r="F90" s="5" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6">
+      <c r="B91" s="3">
+        <v>81</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D91" s="4">
+        <v>44194</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post82
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="251">
   <si>
     <t>S.No</t>
   </si>
@@ -760,6 +760,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/inverted-paging-or-operating-system-m05-p14</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/question-on-inverted-paging-operating-system-m05-p15-4pii</t>
+  </si>
+  <si>
+    <t>Question on Inverted Paging | Operating System - M05 P15</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/question-on-inverted-paging-or-operating-system-m05-p15</t>
   </si>
 </sst>
 </file>
@@ -973,8 +982,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F91" totalsRowShown="0">
-  <autoFilter ref="B10:F91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F92" totalsRowShown="0">
+  <autoFilter ref="B10:F92">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1273,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F91"/>
+  <dimension ref="B10:F92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D82" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2680,6 +2689,23 @@
       </c>
       <c r="F91" s="5" t="s">
         <v>245</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6">
+      <c r="B92" s="3">
+        <v>82</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D92" s="4">
+        <v>44195</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated, with links of Post83
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="254">
   <si>
     <t>S.No</t>
   </si>
@@ -769,6 +769,15 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/question-on-inverted-paging-or-operating-system-m05-p15</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/thrashing-operating-system-m05-p16-463a</t>
+  </si>
+  <si>
+    <t>Thrashing | Operating System - M05 P16</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/thrashing-or-operating-system-m05-p16</t>
   </si>
 </sst>
 </file>
@@ -982,8 +991,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F92" totalsRowShown="0">
-  <autoFilter ref="B10:F92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F93" totalsRowShown="0">
+  <autoFilter ref="B10:F93">
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
@@ -1282,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F92"/>
+  <dimension ref="B10:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D82" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2706,6 +2715,23 @@
       </c>
       <c r="F92" s="5" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6">
+      <c r="B93" s="3">
+        <v>83</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D93" s="4">
+        <v>44196</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated with the links of Post 84
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="259">
   <si>
     <t>S.No</t>
   </si>
@@ -778,6 +778,21 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/thrashing-or-operating-system-m05-p16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File Encrypter and Decrypter </t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/file-encrypter-and-decrypter-10mo</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/file-encrypter-and-decrypter</t>
+  </si>
+  <si>
+    <t>https://thehackedsite.netlify.app/shell/script/2021/03/08/file-encrypter-decrypter</t>
+  </si>
+  <si>
+    <t>Link of Blog Post on The Hacked Site</t>
   </si>
 </sst>
 </file>
@@ -991,16 +1006,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:F93" totalsRowShown="0">
-  <autoFilter ref="B10:F93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G94" totalsRowShown="0">
+  <autoFilter ref="B10:G94">
     <filterColumn colId="4"/>
+    <filterColumn colId="5"/>
   </autoFilter>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" name="S.No"/>
     <tableColumn id="2" name="Title of the Blog Post"/>
     <tableColumn id="3" name="Date of Post" dataDxfId="0"/>
     <tableColumn id="4" name="Link of the Blog Post on Hashnode" dataCellStyle="Hyperlink"/>
     <tableColumn id="5" name="Link of the Blog Post on Dev.to" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" name="Link of Blog Post on The Hacked Site"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1291,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:F93"/>
+  <dimension ref="B10:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D82" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="F88" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1304,9 +1321,10 @@
     <col min="4" max="4" width="17.36328125" customWidth="1"/>
     <col min="5" max="5" width="116" customWidth="1"/>
     <col min="6" max="6" width="133.6328125" customWidth="1"/>
+    <col min="7" max="7" width="86.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:7">
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -1322,8 +1340,11 @@
       <c r="F10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="G10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
       <c r="B11">
         <v>1</v>
       </c>
@@ -1340,7 +1361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:7">
       <c r="B12" s="3">
         <v>2</v>
       </c>
@@ -1357,7 +1378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:7">
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -1374,7 +1395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:7">
       <c r="B14" s="3">
         <v>4</v>
       </c>
@@ -1391,7 +1412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:7">
       <c r="B15" s="3">
         <v>5</v>
       </c>
@@ -1408,7 +1429,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:7">
       <c r="B16" s="3">
         <v>6</v>
       </c>
@@ -2513,7 +2534,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="81" spans="2:6">
+    <row r="81" spans="2:7">
       <c r="B81" s="3">
         <v>71</v>
       </c>
@@ -2530,7 +2551,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="82" spans="2:6">
+    <row r="82" spans="2:7">
       <c r="B82" s="3">
         <v>72</v>
       </c>
@@ -2547,7 +2568,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="83" spans="2:6">
+    <row r="83" spans="2:7">
       <c r="B83" s="3">
         <v>73</v>
       </c>
@@ -2564,7 +2585,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="84" spans="2:6">
+    <row r="84" spans="2:7">
       <c r="B84" s="3">
         <v>74</v>
       </c>
@@ -2581,7 +2602,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="85" spans="2:6">
+    <row r="85" spans="2:7">
       <c r="B85" s="3">
         <v>75</v>
       </c>
@@ -2598,7 +2619,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="86" spans="2:6">
+    <row r="86" spans="2:7">
       <c r="B86" s="3">
         <v>76</v>
       </c>
@@ -2615,7 +2636,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="87" spans="2:6">
+    <row r="87" spans="2:7">
       <c r="B87" s="3">
         <v>77</v>
       </c>
@@ -2632,7 +2653,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="88" spans="2:6">
+    <row r="88" spans="2:7">
       <c r="B88" s="3">
         <v>78</v>
       </c>
@@ -2649,7 +2670,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="89" spans="2:6">
+    <row r="89" spans="2:7">
       <c r="B89" s="3">
         <v>79</v>
       </c>
@@ -2666,7 +2687,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="90" spans="2:6">
+    <row r="90" spans="2:7">
       <c r="B90" s="3">
         <v>80</v>
       </c>
@@ -2683,7 +2704,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="91" spans="2:6">
+    <row r="91" spans="2:7">
       <c r="B91" s="3">
         <v>81</v>
       </c>
@@ -2700,7 +2721,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="92" spans="2:6">
+    <row r="92" spans="2:7">
       <c r="B92" s="3">
         <v>82</v>
       </c>
@@ -2717,7 +2738,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="93" spans="2:6">
+    <row r="93" spans="2:7">
       <c r="B93" s="3">
         <v>83</v>
       </c>
@@ -2732,6 +2753,26 @@
       </c>
       <c r="F93" s="5" t="s">
         <v>251</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7">
+      <c r="B94" s="3">
+        <v>84</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D94" s="4">
+        <v>44263</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G94" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Link of post85 added and .doc file of Post85 completed.
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="263">
   <si>
     <t>S.No</t>
   </si>
@@ -793,6 +793,18 @@
   </si>
   <si>
     <t>Link of Blog Post on The Hacked Site</t>
+  </si>
+  <si>
+    <t>CSRF and SSRF</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/csrf-ssrf-2enp</t>
+  </si>
+  <si>
+    <t>https://thehackedsite.netlify.app/bug/bounty/2021/03/27/csrf-and-ssrf</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/csrf-and-ssrf</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1018,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G94" totalsRowShown="0">
-  <autoFilter ref="B10:G94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G95" totalsRowShown="0">
+  <autoFilter ref="B10:G95">
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
   </autoFilter>
@@ -1308,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:G94"/>
+  <dimension ref="B10:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F88" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" topLeftCell="D74" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2773,6 +2785,26 @@
       </c>
       <c r="G94" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7">
+      <c r="B95" s="3">
+        <v>85</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D95" s="4">
+        <v>44282</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated with links of Post86
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="267">
   <si>
     <t>S.No</t>
   </si>
@@ -805,6 +805,18 @@
   </si>
   <si>
     <t>https://programmingport.hashnode.dev/csrf-and-ssrf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amass: A Beginner's Guide For Reconnaissance </t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/amass-a-beginner-s-guide-for-reconnaissance-4a0p</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/amass-a-beginners-guide-for-reconnaissance</t>
+  </si>
+  <si>
+    <t>https://thehackedsite.netlify.app/bug/bounty/2021/03/28/ammas-a-beginner's-guide-for-reconnaissance</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1030,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G95" totalsRowShown="0">
-  <autoFilter ref="B10:G95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G96" totalsRowShown="0">
+  <autoFilter ref="B10:G96">
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
   </autoFilter>
@@ -1320,10 +1332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:G95"/>
+  <dimension ref="B10:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D74" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="G74" workbookViewId="0">
+      <selection activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1333,7 +1345,7 @@
     <col min="4" max="4" width="17.36328125" customWidth="1"/>
     <col min="5" max="5" width="116" customWidth="1"/>
     <col min="6" max="6" width="133.6328125" customWidth="1"/>
-    <col min="7" max="7" width="86.54296875" customWidth="1"/>
+    <col min="7" max="7" width="95.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="10" spans="2:7">
@@ -2805,6 +2817,26 @@
       </c>
       <c r="G95" s="3" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7">
+      <c r="B96" s="3">
+        <v>86</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D96" s="4">
+        <v>44283</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated with links of Post 87
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="271">
   <si>
     <t>S.No</t>
   </si>
@@ -817,6 +817,18 @@
   </si>
   <si>
     <t>https://thehackedsite.netlify.app/bug/bounty/2021/03/28/ammas-a-beginner's-guide-for-reconnaissance</t>
+  </si>
+  <si>
+    <t>Web Application Penetration Test Checklist | Part - 01</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/web-application-penetration-test-checklist-part-01-4bf</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/web-application-penetration-test-checklist-or-part-01</t>
+  </si>
+  <si>
+    <t>https://thehackedsite.netlify.app/bug/bounty/2021/04/10/web-application-penetration-test-checklist-part-01</t>
   </si>
 </sst>
 </file>
@@ -1030,8 +1042,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G96" totalsRowShown="0">
-  <autoFilter ref="B10:G96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G97" totalsRowShown="0">
+  <autoFilter ref="B10:G97">
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
   </autoFilter>
@@ -1332,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:G96"/>
+  <dimension ref="B10:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G74" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView tabSelected="1" topLeftCell="G86" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2837,6 +2849,26 @@
       </c>
       <c r="G96" s="3" t="s">
         <v>266</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7">
+      <c r="B97" s="3">
+        <v>87</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D97" s="4">
+        <v>44296</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated with the links of Post 88
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="275">
   <si>
     <t>S.No</t>
   </si>
@@ -829,6 +829,18 @@
   </si>
   <si>
     <t>https://thehackedsite.netlify.app/bug/bounty/2021/04/10/web-application-penetration-test-checklist-part-01</t>
+  </si>
+  <si>
+    <t>Web Application Penetration Test Checklist | Part - 02</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/web-application-penetration-test-checklist-part-02-1igc</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/web-application-penetration-test-checklist-or-part-02</t>
+  </si>
+  <si>
+    <t>https://thehackedsite.netlify.app/bug/bounty/2021/04/11/web-application-penetration-test-checklist-part-02</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1054,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G97" totalsRowShown="0">
-  <autoFilter ref="B10:G97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G98" totalsRowShown="0">
+  <autoFilter ref="B10:G98">
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
   </autoFilter>
@@ -1344,7 +1356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:G97"/>
+  <dimension ref="B10:G98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G86" workbookViewId="0">
       <selection activeCell="G98" sqref="G98"/>
@@ -2869,6 +2881,26 @@
       </c>
       <c r="G97" s="3" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7">
+      <c r="B98" s="3">
+        <v>88</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D98" s="4">
+        <v>44297</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log file updated with links of Post 89.
</commit_message>
<xml_diff>
--- a/Log_of_all_Blogs.xlsx
+++ b/Log_of_all_Blogs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="278">
   <si>
     <t>S.No</t>
   </si>
@@ -841,6 +841,15 @@
   </si>
   <si>
     <t>https://thehackedsite.netlify.app/bug/bounty/2021/04/11/web-application-penetration-test-checklist-part-02</t>
+  </si>
+  <si>
+    <t>https://dev.to/rahulmishra05/broken-authentication-methodology-prevention-33nd</t>
+  </si>
+  <si>
+    <t>https://programmingport.hashnode.dev/broken-authentication-methodology-and-prevention</t>
+  </si>
+  <si>
+    <t>https://thehackedsite.netlify.app/bug/bounty/2021/05/12/broken-authentication-methodology-and-prevention</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1063,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G98" totalsRowShown="0">
-  <autoFilter ref="B10:G98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B10:G99" totalsRowShown="0">
+  <autoFilter ref="B10:G99">
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
   </autoFilter>
@@ -1356,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B10:G98"/>
+  <dimension ref="B10:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G86" workbookViewId="0">
-      <selection activeCell="G98" sqref="G98"/>
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2901,6 +2910,22 @@
       </c>
       <c r="G98" s="3" t="s">
         <v>274</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7">
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="4">
+        <v>44328</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>